<commit_message>
implementation of export pdf in laravel with dompdf
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85951BD5-5164-4A4C-8541-EAFFC57917CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BDDCA1-B0AC-49E1-BEB9-714DA8A6C420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -37,21 +37,6 @@
     <t>harga_jual</t>
   </si>
   <si>
-    <t>BRG0011</t>
-  </si>
-  <si>
-    <t>BRG0012</t>
-  </si>
-  <si>
-    <t>BRG0013</t>
-  </si>
-  <si>
-    <t>BRG0014</t>
-  </si>
-  <si>
-    <t>BRG0015</t>
-  </si>
-  <si>
     <t>Smartwatch Apple</t>
   </si>
   <si>
@@ -65,6 +50,21 @@
   </si>
   <si>
     <t>Penggaris</t>
+  </si>
+  <si>
+    <t>BRG011</t>
+  </si>
+  <si>
+    <t>BRG012</t>
+  </si>
+  <si>
+    <t>BRG013</t>
+  </si>
+  <si>
+    <t>BRG014</t>
+  </si>
+  <si>
+    <t>BRG015</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,10 +453,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
       <c r="D2">
         <v>5500000</v>
@@ -470,10 +470,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>125000</v>
@@ -487,10 +487,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
       <c r="D4">
         <v>8000</v>
@@ -504,10 +504,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
       <c r="D5">
         <v>20000</v>
@@ -521,10 +521,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
       <c r="D6">
         <v>3000</v>

</xml_diff>